<commit_message>
add change interface and date
</commit_message>
<xml_diff>
--- a/project/Tabla1.xlsx
+++ b/project/Tabla1.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -732,348 +732,6 @@
         <v>834</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>ISSFA - 0045</t>
-        </is>
-      </c>
-      <c r="B6" s="2" t="n">
-        <v>44220</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Iñaquito</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Quito</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Quito</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Quito</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Pichincha</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>Casa</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>Horizontal</t>
-        </is>
-      </c>
-      <c r="J6" t="n">
-        <v>523</v>
-      </c>
-      <c r="K6" t="n">
-        <v>834</v>
-      </c>
-      <c r="L6" t="n">
-        <v>750.6</v>
-      </c>
-      <c r="M6" t="n">
-        <v>834</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>ISSFA - 0045</t>
-        </is>
-      </c>
-      <c r="B7" s="2" t="n">
-        <v>44220</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Iñaquito</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Quito</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Quito</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Quito</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>Pichincha</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>Casa</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>Horizontal</t>
-        </is>
-      </c>
-      <c r="J7" t="n">
-        <v>523</v>
-      </c>
-      <c r="K7" t="n">
-        <v>834</v>
-      </c>
-      <c r="L7" t="n">
-        <v>750.6</v>
-      </c>
-      <c r="M7" t="n">
-        <v>834</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>ISSFA - 0045</t>
-        </is>
-      </c>
-      <c r="B8" s="2" t="n">
-        <v>44220</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Iñaquito</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Quito</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Quito</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>Quito</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>Pichincha</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>Casa</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>Horizontal</t>
-        </is>
-      </c>
-      <c r="J8" t="n">
-        <v>523</v>
-      </c>
-      <c r="K8" t="n">
-        <v>834</v>
-      </c>
-      <c r="L8" t="n">
-        <v>750.6</v>
-      </c>
-      <c r="M8" t="n">
-        <v>834</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>ISSFA - 0045</t>
-        </is>
-      </c>
-      <c r="B9" s="2" t="n">
-        <v>44220</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Iñaquito</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Quito</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Quito</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>Quito</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>Pichincha</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>Casa</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>Horizontal</t>
-        </is>
-      </c>
-      <c r="J9" t="n">
-        <v>523</v>
-      </c>
-      <c r="K9" t="n">
-        <v>834</v>
-      </c>
-      <c r="L9" t="n">
-        <v>750.6</v>
-      </c>
-      <c r="M9" t="n">
-        <v>834</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>ISSFA - 0045</t>
-        </is>
-      </c>
-      <c r="B10" s="2" t="n">
-        <v>44220</v>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Iñaquito</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Quito</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Quito</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>Quito</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>Pichincha</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>Casa</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>Horizontal</t>
-        </is>
-      </c>
-      <c r="J10" t="n">
-        <v>523</v>
-      </c>
-      <c r="K10" t="n">
-        <v>834</v>
-      </c>
-      <c r="L10" t="n">
-        <v>750.6</v>
-      </c>
-      <c r="M10" t="n">
-        <v>834</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>ISSFA - 0045</t>
-        </is>
-      </c>
-      <c r="B11" s="2" t="n">
-        <v>44220</v>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Iñaquito</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Quito</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Quito</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>Quito</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>Pichincha</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>Casa</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>Horizontal</t>
-        </is>
-      </c>
-      <c r="J11" t="n">
-        <v>523</v>
-      </c>
-      <c r="K11" t="n">
-        <v>834</v>
-      </c>
-      <c r="L11" t="n">
-        <v>750.6</v>
-      </c>
-      <c r="M11" t="n">
-        <v>834</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
add change to run exe
</commit_message>
<xml_diff>
--- a/project/Tabla1.xlsx
+++ b/project/Tabla1.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -846,6 +846,63 @@
         <v>834</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>ISSFA - 0045</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>44220</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Iñaquito</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Quito</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Quito</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Quito</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Pichincha</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Casa</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Horizontal</t>
+        </is>
+      </c>
+      <c r="J8" t="n">
+        <v>523</v>
+      </c>
+      <c r="K8" t="n">
+        <v>834</v>
+      </c>
+      <c r="L8" t="n">
+        <v>750.6</v>
+      </c>
+      <c r="M8" t="n">
+        <v>834</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
change lenght of views
</commit_message>
<xml_diff>
--- a/project/Tabla1.xlsx
+++ b/project/Tabla1.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -903,6 +903,63 @@
         <v>834</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>ISSFA - 0045</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>44220</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Iñaquito</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Quito</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Quito</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Quito</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Pichincha</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Casa</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Horizontal</t>
+        </is>
+      </c>
+      <c r="J9" t="n">
+        <v>523</v>
+      </c>
+      <c r="K9" t="n">
+        <v>834</v>
+      </c>
+      <c r="L9" t="n">
+        <v>750.6</v>
+      </c>
+      <c r="M9" t="n">
+        <v>834</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
add changes in the pichincha
</commit_message>
<xml_diff>
--- a/project/Tabla1.xlsx
+++ b/project/Tabla1.xlsx
@@ -1,87 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jazmin Rodriguez\Desktop\Proyectos GitHub\PYQT-Interface-gen-access-DataBase\project\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AEE61AE-0E7E-4D7B-939D-E2351FD02E37}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="1845" yWindow="495" windowWidth="18645" windowHeight="11025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>NUA</t>
-  </si>
-  <si>
-    <t>FECHA</t>
-  </si>
-  <si>
-    <t>SECTOR</t>
-  </si>
-  <si>
-    <t>PARROQUIA</t>
-  </si>
-  <si>
-    <t>CIUDAD</t>
-  </si>
-  <si>
-    <t>CANTON</t>
-  </si>
-  <si>
-    <t>PROVINCIA</t>
-  </si>
-  <si>
-    <t>INMUEBLE</t>
-  </si>
-  <si>
-    <t>REGIMEN DE PROPIEDAD</t>
-  </si>
-  <si>
-    <t>AREA TERRENO</t>
-  </si>
-  <si>
-    <t>VALOR UNITARIO x M2</t>
-  </si>
-  <si>
-    <t>AVALUO TOTAL</t>
-  </si>
-  <si>
-    <t>VALOR DE LA REALIZACION</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="164"/>
+    <numFmt formatCode="YYYY-MM-DD HH:MM:SS" numFmtId="165"/>
+  </numFmts>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -96,43 +49,94 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="3">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -420,60 +424,144 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="31.42578125" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>NUA</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>FECHA</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>SECTOR</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>PARROQUIA</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>CIUDAD</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>CANTON</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>PROVINCIA</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>INMUEBLE</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>REGIMEN DE PROPIEDAD</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>AREA TERRENO</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>VALOR UNITARIO x M2</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>AVALUO TOTAL</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>VALOR DE LA REALIZACION</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>ISSFA - 0045</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>44220</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Iñaquito</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Quito</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Quito</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Quito</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Pichincha</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Casa</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Horizontal</t>
+        </is>
+      </c>
+      <c r="J2" t="n">
+        <v>523</v>
+      </c>
+      <c r="K2" t="n">
+        <v>834</v>
+      </c>
+      <c r="L2" t="n">
+        <v>750.6</v>
+      </c>
+      <c r="M2" t="n">
+        <v>834</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>